<commit_message>
update excel sheet name
</commit_message>
<xml_diff>
--- a/public/templates/att_report-2.xlsx
+++ b/public/templates/att_report-2.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\meir-att\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4314FE0F-5C44-4795-9C98-5E314138C1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247505B8-A159-427C-BB5E-1752757DFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21900" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
   <sheets>
-    <sheet name="גליון" sheetId="1" r:id="rId1"/>
+    <sheet name="דצמבר" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>

<commit_message>
add teacher name & klass & lesson to excel file
</commit_message>
<xml_diff>
--- a/public/templates/att_report-2.xlsx
+++ b/public/templates/att_report-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\meir-att\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247505B8-A159-427C-BB5E-1752757DFFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B48C2F-8CF2-4E75-A58A-1F5F8C28BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="21900" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ת.ז.</t>
   </si>
@@ -69,6 +61,15 @@
   </si>
   <si>
     <t>חיסורים או ציונים</t>
+  </si>
+  <si>
+    <t>${lesson.klass.name}</t>
+  </si>
+  <si>
+    <t>${lesson.teacher.name}</t>
+  </si>
+  <si>
+    <t>${lesson.name}</t>
   </si>
 </sst>
 </file>
@@ -128,10 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F0D8B3-8917-4C0C-99DA-1853A0CA42E9}">
-  <dimension ref="A1:G314"/>
+  <dimension ref="A1:H315"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -463,7 +465,7 @@
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -486,63 +488,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1438,6 +1453,9 @@
     </row>
     <row r="314" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B314" s="2"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B315" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix teacher fetching - fetch by user_id
</commit_message>
<xml_diff>
--- a/public/templates/att_report-2.xlsx
+++ b/public/templates/att_report-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\SideProjects\report-projects\meir-att\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B48C2F-8CF2-4E75-A58A-1F5F8C28BE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C93BBE8-762F-44CC-BE91-4E3257D80777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="21900" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21960" windowHeight="13176" xr2:uid="{2F61205C-6BC3-4C3D-9F5C-D8E7A2EA9148}"/>
   </bookViews>
   <sheets>
     <sheet name="דצמבר" sheetId="1" r:id="rId1"/>
@@ -63,13 +63,13 @@
     <t>חיסורים או ציונים</t>
   </si>
   <si>
-    <t>${lesson.klass.name}</t>
+    <t>${lesson.name}</t>
   </si>
   <si>
-    <t>${lesson.teacher.name}</t>
+    <t>${teacher.name}</t>
   </si>
   <si>
-    <t>${lesson.name}</t>
+    <t>${klass.name}</t>
   </si>
 </sst>
 </file>
@@ -440,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -451,7 +451,7 @@
   <dimension ref="A1:H315"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -490,7 +490,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -498,7 +498,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>

</xml_diff>